<commit_message>
Sphere Minor: - Speaker positions - Sample Frequency - Miscellaneous
</commit_message>
<xml_diff>
--- a/experiment/sphereMinor/setup/SphereMinor Measurement.xlsx
+++ b/experiment/sphereMinor/setup/SphereMinor Measurement.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jasper\Documents\MATLAB\biofysica-master-141af8ba805977bde67ecf7b5c4f21c76af98056\experiment\sphereMinor\setup\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8085" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Diagram" sheetId="2" r:id="rId1"/>
     <sheet name="Values" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -43,8 +48,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -95,11 +100,6 @@
       <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -975,7 +975,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1346,12 +1346,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1386,90 +1380,77 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1447800" y="4581525"/>
+          <a:ext cx="8648700" cy="6219825"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1794,18 +1775,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AX35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="4.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="4.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:50" ht="34">
+    <row r="1" spans="1:50" ht="32.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1957,7 +1938,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:50">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>120</v>
       </c>
@@ -2017,7 +1998,7 @@
       <c r="AW2" s="3"/>
       <c r="AX2" s="3"/>
     </row>
-    <row r="3" spans="1:50">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>115</v>
       </c>
@@ -2071,7 +2052,7 @@
       <c r="AW3" s="3"/>
       <c r="AX3" s="3"/>
     </row>
-    <row r="4" spans="1:50">
+    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>110</v>
       </c>
@@ -2125,7 +2106,7 @@
       <c r="AW4" s="3"/>
       <c r="AX4" s="3"/>
     </row>
-    <row r="5" spans="1:50">
+    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>105</v>
       </c>
@@ -2181,7 +2162,7 @@
       <c r="AW5" s="3"/>
       <c r="AX5" s="3"/>
     </row>
-    <row r="6" spans="1:50">
+    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>100</v>
       </c>
@@ -2235,7 +2216,7 @@
       <c r="AW6" s="3"/>
       <c r="AX6" s="3"/>
     </row>
-    <row r="7" spans="1:50">
+    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>95</v>
       </c>
@@ -2289,7 +2270,7 @@
       <c r="AW7" s="3"/>
       <c r="AX7" s="3"/>
     </row>
-    <row r="8" spans="1:50">
+    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>90</v>
       </c>
@@ -2345,7 +2326,7 @@
       <c r="AW8" s="3"/>
       <c r="AX8" s="3"/>
     </row>
-    <row r="9" spans="1:50">
+    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>85</v>
       </c>
@@ -2399,7 +2380,7 @@
       <c r="AW9" s="3"/>
       <c r="AX9" s="3"/>
     </row>
-    <row r="10" spans="1:50">
+    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>80</v>
       </c>
@@ -2453,7 +2434,7 @@
       <c r="AW10" s="3"/>
       <c r="AX10" s="3"/>
     </row>
-    <row r="11" spans="1:50">
+    <row r="11" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>75</v>
       </c>
@@ -2513,7 +2494,7 @@
       <c r="AW11" s="3"/>
       <c r="AX11" s="3"/>
     </row>
-    <row r="12" spans="1:50">
+    <row r="12" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>70</v>
       </c>
@@ -2567,7 +2548,7 @@
       <c r="AW12" s="3"/>
       <c r="AX12" s="3"/>
     </row>
-    <row r="13" spans="1:50">
+    <row r="13" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>65</v>
       </c>
@@ -2621,7 +2602,7 @@
       <c r="AW13" s="3"/>
       <c r="AX13" s="3"/>
     </row>
-    <row r="14" spans="1:50">
+    <row r="14" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>60</v>
       </c>
@@ -2685,7 +2666,7 @@
       <c r="AW14" s="3"/>
       <c r="AX14" s="3"/>
     </row>
-    <row r="15" spans="1:50">
+    <row r="15" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>55</v>
       </c>
@@ -2739,7 +2720,7 @@
       <c r="AW15" s="3"/>
       <c r="AX15" s="3"/>
     </row>
-    <row r="16" spans="1:50">
+    <row r="16" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>50</v>
       </c>
@@ -2793,7 +2774,7 @@
       <c r="AW16" s="3"/>
       <c r="AX16" s="3"/>
     </row>
-    <row r="17" spans="1:50">
+    <row r="17" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>45</v>
       </c>
@@ -2861,7 +2842,7 @@
       <c r="AW17" s="3"/>
       <c r="AX17" s="3"/>
     </row>
-    <row r="18" spans="1:50">
+    <row r="18" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>40</v>
       </c>
@@ -2917,7 +2898,7 @@
       <c r="AW18" s="3"/>
       <c r="AX18" s="3"/>
     </row>
-    <row r="19" spans="1:50">
+    <row r="19" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>35</v>
       </c>
@@ -2973,7 +2954,7 @@
       <c r="AW19" s="3"/>
       <c r="AX19" s="3"/>
     </row>
-    <row r="20" spans="1:50">
+    <row r="20" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>30</v>
       </c>
@@ -3045,7 +3026,7 @@
       <c r="AW20" s="3"/>
       <c r="AX20" s="3"/>
     </row>
-    <row r="21" spans="1:50">
+    <row r="21" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>25</v>
       </c>
@@ -3101,7 +3082,7 @@
       <c r="AW21" s="3"/>
       <c r="AX21" s="3"/>
     </row>
-    <row r="22" spans="1:50">
+    <row r="22" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -3157,7 +3138,7 @@
       <c r="AW22" s="3"/>
       <c r="AX22" s="3"/>
     </row>
-    <row r="23" spans="1:50">
+    <row r="23" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>15</v>
       </c>
@@ -3237,7 +3218,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="24" spans="1:50">
+    <row r="24" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>10</v>
       </c>
@@ -3293,7 +3274,7 @@
       <c r="AW24" s="3"/>
       <c r="AX24" s="3"/>
     </row>
-    <row r="25" spans="1:50">
+    <row r="25" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>5</v>
       </c>
@@ -3349,7 +3330,7 @@
       <c r="AW25" s="3"/>
       <c r="AX25" s="3"/>
     </row>
-    <row r="26" spans="1:50">
+    <row r="26" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>0</v>
       </c>
@@ -3461,7 +3442,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:50">
+    <row r="27" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>-5</v>
       </c>
@@ -3517,7 +3498,7 @@
       <c r="AW27" s="3"/>
       <c r="AX27" s="3"/>
     </row>
-    <row r="28" spans="1:50">
+    <row r="28" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>-10</v>
       </c>
@@ -3573,7 +3554,7 @@
       <c r="AW28" s="3"/>
       <c r="AX28" s="3"/>
     </row>
-    <row r="29" spans="1:50">
+    <row r="29" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>-15</v>
       </c>
@@ -3653,7 +3634,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="30" spans="1:50">
+    <row r="30" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>-20</v>
       </c>
@@ -3709,7 +3690,7 @@
       <c r="AW30" s="3"/>
       <c r="AX30" s="3"/>
     </row>
-    <row r="31" spans="1:50">
+    <row r="31" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>-25</v>
       </c>
@@ -3765,7 +3746,7 @@
       <c r="AW31" s="3"/>
       <c r="AX31" s="3"/>
     </row>
-    <row r="32" spans="1:50">
+    <row r="32" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>-30</v>
       </c>
@@ -3837,7 +3818,7 @@
       <c r="AW32" s="3"/>
       <c r="AX32" s="3"/>
     </row>
-    <row r="33" spans="1:50">
+    <row r="33" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>-35</v>
       </c>
@@ -3893,7 +3874,7 @@
       <c r="AW33" s="3"/>
       <c r="AX33" s="3"/>
     </row>
-    <row r="34" spans="1:50">
+    <row r="34" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>-40</v>
       </c>
@@ -3949,7 +3930,7 @@
       <c r="AW34" s="3"/>
       <c r="AX34" s="3"/>
     </row>
-    <row r="35" spans="1:50">
+    <row r="35" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>-45</v>
       </c>
@@ -4020,7 +4001,8 @@
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" scale="52" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" scale="52" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>
@@ -4033,16 +4015,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39:E39"/>
+    <sheetView topLeftCell="A55" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32:E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="123"/>
+    <col min="1" max="16384" width="10.875" style="123"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16" thickBot="1">
+    <row r="1" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="118" t="s">
         <v>0</v>
       </c>
@@ -4059,1909 +4041,1085 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="124">
         <v>0</v>
       </c>
       <c r="B2" s="116">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="C2" s="125">
         <v>0</v>
       </c>
-      <c r="D2" s="126">
-        <v>-126</v>
-      </c>
-      <c r="E2" s="127">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="D2" s="116">
+        <v>0</v>
+      </c>
+      <c r="E2" s="125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="124">
-        <v>96</v>
+        <v>1</v>
       </c>
       <c r="B3" s="116">
-        <v>-120</v>
+        <v>-10</v>
       </c>
       <c r="C3" s="125">
-        <v>-15</v>
-      </c>
-      <c r="D3" s="126">
-        <v>-123</v>
-      </c>
-      <c r="E3" s="127">
-        <v>-13.7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>0</v>
+      </c>
+      <c r="D3" s="116">
+        <v>-10</v>
+      </c>
+      <c r="E3" s="125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="124">
-        <v>97</v>
+        <v>2</v>
       </c>
       <c r="B4" s="116">
-        <v>-120</v>
+        <v>-20</v>
       </c>
       <c r="C4" s="125">
+        <v>0</v>
+      </c>
+      <c r="D4" s="116">
+        <v>-20</v>
+      </c>
+      <c r="E4" s="125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="124">
+        <v>3</v>
+      </c>
+      <c r="B5" s="116">
+        <v>-30</v>
+      </c>
+      <c r="C5" s="125">
+        <v>0</v>
+      </c>
+      <c r="D5" s="116">
+        <v>-30</v>
+      </c>
+      <c r="E5" s="125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="124">
+        <v>4</v>
+      </c>
+      <c r="B6" s="116">
+        <v>-40</v>
+      </c>
+      <c r="C6" s="125">
+        <v>0</v>
+      </c>
+      <c r="D6" s="116">
+        <v>-40</v>
+      </c>
+      <c r="E6" s="125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="124">
+        <v>5</v>
+      </c>
+      <c r="B7" s="116">
+        <v>-50</v>
+      </c>
+      <c r="C7" s="125">
+        <v>0</v>
+      </c>
+      <c r="D7" s="116">
+        <v>-50</v>
+      </c>
+      <c r="E7" s="125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="124">
+        <v>6</v>
+      </c>
+      <c r="B8" s="116">
+        <v>-60</v>
+      </c>
+      <c r="C8" s="125">
+        <v>0</v>
+      </c>
+      <c r="D8" s="116">
+        <v>-60</v>
+      </c>
+      <c r="E8" s="125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="124">
+        <v>7</v>
+      </c>
+      <c r="B9" s="116">
+        <v>-70</v>
+      </c>
+      <c r="C9" s="125">
+        <v>0</v>
+      </c>
+      <c r="D9" s="116">
+        <v>-70</v>
+      </c>
+      <c r="E9" s="125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="124">
+        <v>8</v>
+      </c>
+      <c r="B10" s="116">
+        <v>-80</v>
+      </c>
+      <c r="C10" s="125">
+        <v>0</v>
+      </c>
+      <c r="D10" s="116">
+        <v>-80</v>
+      </c>
+      <c r="E10" s="125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="124">
+        <v>9</v>
+      </c>
+      <c r="B11" s="116">
+        <v>-90</v>
+      </c>
+      <c r="C11" s="125">
+        <v>0</v>
+      </c>
+      <c r="D11" s="116">
+        <v>-90</v>
+      </c>
+      <c r="E11" s="125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="124">
+        <v>10</v>
+      </c>
+      <c r="B12" s="116">
+        <v>0</v>
+      </c>
+      <c r="C12" s="125">
+        <v>10</v>
+      </c>
+      <c r="D12" s="116">
+        <v>0</v>
+      </c>
+      <c r="E12" s="125">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="124">
+        <v>11</v>
+      </c>
+      <c r="B13" s="116">
+        <v>0</v>
+      </c>
+      <c r="C13" s="125">
+        <v>20</v>
+      </c>
+      <c r="D13" s="116">
+        <v>0</v>
+      </c>
+      <c r="E13" s="125">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="124">
+        <v>12</v>
+      </c>
+      <c r="B14" s="116">
+        <v>0</v>
+      </c>
+      <c r="C14" s="125">
+        <v>30</v>
+      </c>
+      <c r="D14" s="116">
+        <v>0</v>
+      </c>
+      <c r="E14" s="125">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="124">
+        <v>13</v>
+      </c>
+      <c r="B15" s="116">
+        <v>0</v>
+      </c>
+      <c r="C15" s="125">
+        <v>40</v>
+      </c>
+      <c r="D15" s="116">
+        <v>0</v>
+      </c>
+      <c r="E15" s="125">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="124">
+        <v>14</v>
+      </c>
+      <c r="B16" s="116">
+        <v>0</v>
+      </c>
+      <c r="C16" s="125">
+        <v>50</v>
+      </c>
+      <c r="D16" s="116">
+        <v>0</v>
+      </c>
+      <c r="E16" s="125">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="124">
         <v>15</v>
       </c>
-      <c r="D4" s="126">
-        <v>-121</v>
-      </c>
-      <c r="E4" s="127">
-        <v>15.25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="124">
-        <v>32</v>
-      </c>
-      <c r="B5" s="116">
-        <v>-105</v>
-      </c>
-      <c r="C5" s="125">
-        <v>0</v>
-      </c>
-      <c r="D5" s="117">
-        <v>-110</v>
-      </c>
-      <c r="E5" s="128">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="124">
-        <v>1</v>
-      </c>
-      <c r="B6" s="116">
-        <v>-90</v>
-      </c>
-      <c r="C6" s="125">
-        <v>0</v>
-      </c>
-      <c r="D6" s="117">
-        <v>-95</v>
-      </c>
-      <c r="E6" s="128">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="124">
-        <v>33</v>
-      </c>
-      <c r="B7" s="116">
-        <v>-75</v>
-      </c>
-      <c r="C7" s="125">
-        <v>0</v>
-      </c>
-      <c r="D7" s="117">
-        <v>-79.5</v>
-      </c>
-      <c r="E7" s="128">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="124">
-        <v>64</v>
-      </c>
-      <c r="B8" s="116">
-        <v>-75</v>
-      </c>
-      <c r="C8" s="125">
-        <v>-15</v>
-      </c>
-      <c r="D8" s="117">
-        <v>-94.5</v>
-      </c>
-      <c r="E8" s="128">
-        <v>-14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="124">
-        <v>65</v>
-      </c>
-      <c r="B9" s="116">
-        <v>-75</v>
-      </c>
-      <c r="C9" s="125">
-        <v>15</v>
-      </c>
-      <c r="D9" s="117">
-        <v>-94.5</v>
-      </c>
-      <c r="E9" s="128">
-        <v>14.6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="124">
-        <v>2</v>
-      </c>
-      <c r="B10" s="116">
-        <v>-60</v>
-      </c>
-      <c r="C10" s="125">
+      <c r="B17" s="116">
+        <v>0</v>
+      </c>
+      <c r="C17" s="125">
+        <v>60</v>
+      </c>
+      <c r="D17" s="116">
+        <v>0</v>
+      </c>
+      <c r="E17" s="125">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="124">
+        <v>16</v>
+      </c>
+      <c r="B18" s="116"/>
+      <c r="C18" s="125"/>
+      <c r="D18" s="116"/>
+      <c r="E18" s="125"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="124">
+        <v>17</v>
+      </c>
+      <c r="B19" s="116">
+        <v>10</v>
+      </c>
+      <c r="C19" s="125">
+        <v>0</v>
+      </c>
+      <c r="D19" s="116">
+        <v>10</v>
+      </c>
+      <c r="E19" s="125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="124">
+        <v>18</v>
+      </c>
+      <c r="B20" s="116">
+        <v>20</v>
+      </c>
+      <c r="C20" s="125">
+        <v>0</v>
+      </c>
+      <c r="D20" s="116">
+        <v>20</v>
+      </c>
+      <c r="E20" s="125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="124">
+        <v>19</v>
+      </c>
+      <c r="B21" s="116">
+        <v>30</v>
+      </c>
+      <c r="C21" s="125">
+        <v>0</v>
+      </c>
+      <c r="D21" s="116">
+        <v>30</v>
+      </c>
+      <c r="E21" s="125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="124">
+        <v>20</v>
+      </c>
+      <c r="B22" s="116">
+        <v>40</v>
+      </c>
+      <c r="C22" s="125">
+        <v>0</v>
+      </c>
+      <c r="D22" s="116">
+        <v>40</v>
+      </c>
+      <c r="E22" s="125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="124">
+        <v>21</v>
+      </c>
+      <c r="B23" s="116">
+        <v>50</v>
+      </c>
+      <c r="C23" s="125">
+        <v>0</v>
+      </c>
+      <c r="D23" s="116">
+        <v>50</v>
+      </c>
+      <c r="E23" s="125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="124">
+        <v>22</v>
+      </c>
+      <c r="B24" s="116">
+        <v>60</v>
+      </c>
+      <c r="C24" s="125">
+        <v>0</v>
+      </c>
+      <c r="D24" s="116">
+        <v>60</v>
+      </c>
+      <c r="E24" s="125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="124">
+        <v>23</v>
+      </c>
+      <c r="B25" s="116">
+        <v>70</v>
+      </c>
+      <c r="C25" s="125">
+        <v>0</v>
+      </c>
+      <c r="D25" s="116">
+        <v>70</v>
+      </c>
+      <c r="E25" s="125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="124">
+        <v>24</v>
+      </c>
+      <c r="B26" s="116">
+        <v>80</v>
+      </c>
+      <c r="C26" s="125">
+        <v>0</v>
+      </c>
+      <c r="D26" s="116">
+        <v>80</v>
+      </c>
+      <c r="E26" s="125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="124">
+        <v>25</v>
+      </c>
+      <c r="B27" s="116">
+        <v>90</v>
+      </c>
+      <c r="C27" s="125">
+        <v>0</v>
+      </c>
+      <c r="D27" s="116">
+        <v>90</v>
+      </c>
+      <c r="E27" s="125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="124">
+        <v>26</v>
+      </c>
+      <c r="B28" s="116">
+        <v>0</v>
+      </c>
+      <c r="C28" s="125">
+        <v>-10</v>
+      </c>
+      <c r="D28" s="116">
+        <v>0</v>
+      </c>
+      <c r="E28" s="125">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="124">
+        <v>27</v>
+      </c>
+      <c r="B29" s="116">
+        <v>0</v>
+      </c>
+      <c r="C29" s="125">
+        <v>-20</v>
+      </c>
+      <c r="D29" s="116">
+        <v>0</v>
+      </c>
+      <c r="E29" s="125">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="124">
+        <v>28</v>
+      </c>
+      <c r="B30" s="116">
+        <v>0</v>
+      </c>
+      <c r="C30" s="125">
         <v>-30</v>
       </c>
-      <c r="D10" s="117">
-        <v>-95</v>
-      </c>
-      <c r="E10" s="128">
-        <v>-29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="124">
-        <v>3</v>
-      </c>
-      <c r="B11" s="116">
-        <v>-60</v>
-      </c>
-      <c r="C11" s="125">
-        <v>0</v>
-      </c>
-      <c r="D11" s="117">
-        <v>-64</v>
-      </c>
-      <c r="E11" s="128">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="124">
-        <v>4</v>
-      </c>
-      <c r="B12" s="116">
-        <v>-60</v>
-      </c>
-      <c r="C12" s="125">
+      <c r="D30" s="116">
+        <v>0</v>
+      </c>
+      <c r="E30" s="125">
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="124">
+        <v>29</v>
+      </c>
+      <c r="B31" s="116">
+        <v>0</v>
+      </c>
+      <c r="C31" s="125">
+        <v>-40</v>
+      </c>
+      <c r="D31" s="116">
+        <v>0</v>
+      </c>
+      <c r="E31" s="125">
+        <v>-40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="124">
         <v>30</v>
       </c>
-      <c r="D12" s="117">
-        <v>-93</v>
-      </c>
-      <c r="E12" s="128">
-        <v>30.3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="124">
-        <v>98</v>
-      </c>
-      <c r="B13" s="116">
-        <v>-60</v>
-      </c>
-      <c r="C13" s="125">
-        <v>-15</v>
-      </c>
-      <c r="D13" s="117">
-        <v>-67.5</v>
-      </c>
-      <c r="E13" s="128">
-        <v>-14.3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="124">
-        <v>99</v>
-      </c>
-      <c r="B14" s="116">
-        <v>-60</v>
-      </c>
-      <c r="C14" s="125">
-        <v>15</v>
-      </c>
-      <c r="D14" s="117">
-        <v>-63</v>
-      </c>
-      <c r="E14" s="128">
-        <v>15.6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="124">
-        <v>34</v>
-      </c>
-      <c r="B15" s="116">
-        <v>-45</v>
-      </c>
-      <c r="C15" s="125">
-        <v>-30</v>
-      </c>
-      <c r="D15" s="117">
-        <v>-59.5</v>
-      </c>
-      <c r="E15" s="128">
-        <v>-29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="124">
-        <v>35</v>
-      </c>
-      <c r="B16" s="116">
-        <v>-45</v>
-      </c>
-      <c r="C16" s="125">
-        <v>0</v>
-      </c>
-      <c r="D16" s="117">
-        <v>-45</v>
-      </c>
-      <c r="E16" s="128">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="124">
-        <v>36</v>
-      </c>
-      <c r="B17" s="116">
-        <v>-45</v>
-      </c>
-      <c r="C17" s="125">
-        <v>30</v>
-      </c>
-      <c r="D17" s="117">
-        <v>-57</v>
-      </c>
-      <c r="E17" s="128">
-        <v>29.2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="124">
-        <v>66</v>
-      </c>
-      <c r="B18" s="116">
-        <v>-45</v>
-      </c>
-      <c r="C18" s="125">
-        <v>-45</v>
-      </c>
-      <c r="D18" s="117">
-        <v>-74.5</v>
-      </c>
-      <c r="E18" s="128">
-        <v>-41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="124">
-        <v>67</v>
-      </c>
-      <c r="B19" s="116">
-        <v>-45</v>
-      </c>
-      <c r="C19" s="125">
-        <v>-15</v>
-      </c>
-      <c r="D19" s="117">
-        <v>-51</v>
-      </c>
-      <c r="E19" s="128">
-        <v>-14.7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="124">
-        <v>68</v>
-      </c>
-      <c r="B20" s="116">
-        <v>-45</v>
-      </c>
-      <c r="C20" s="125">
-        <v>15</v>
-      </c>
-      <c r="D20" s="117">
-        <v>-51</v>
-      </c>
-      <c r="E20" s="128">
-        <v>15.9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="124">
-        <v>69</v>
-      </c>
-      <c r="B21" s="116">
-        <v>-45</v>
-      </c>
-      <c r="C21" s="125">
-        <v>45</v>
-      </c>
-      <c r="D21" s="117">
-        <v>-75.5</v>
-      </c>
-      <c r="E21" s="128">
-        <v>41.3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="124">
-        <v>84</v>
-      </c>
-      <c r="B22" s="116">
-        <v>-40</v>
-      </c>
-      <c r="C22" s="125">
-        <v>0</v>
-      </c>
-      <c r="D22" s="117">
-        <v>-40</v>
-      </c>
-      <c r="E22" s="128">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="124">
-        <v>118</v>
-      </c>
-      <c r="B23" s="116">
-        <v>-35</v>
-      </c>
-      <c r="C23" s="125">
-        <v>0</v>
-      </c>
-      <c r="D23" s="117">
-        <v>-35</v>
-      </c>
-      <c r="E23" s="128">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="124">
-        <v>5</v>
-      </c>
-      <c r="B24" s="116">
-        <v>-30</v>
-      </c>
-      <c r="C24" s="125">
-        <v>-30</v>
-      </c>
-      <c r="D24" s="117">
-        <v>-38</v>
-      </c>
-      <c r="E24" s="128">
-        <v>-28.8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="124">
-        <v>6</v>
-      </c>
-      <c r="B25" s="116">
-        <v>-30</v>
-      </c>
-      <c r="C25" s="125">
-        <v>0</v>
-      </c>
-      <c r="D25" s="117">
-        <v>-30</v>
-      </c>
-      <c r="E25" s="128">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="124">
-        <v>7</v>
-      </c>
-      <c r="B26" s="116">
-        <v>-30</v>
-      </c>
-      <c r="C26" s="125">
-        <v>30</v>
-      </c>
-      <c r="D26" s="117">
-        <v>-39</v>
-      </c>
-      <c r="E26" s="128">
-        <v>30.5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="124">
-        <v>8</v>
-      </c>
-      <c r="B27" s="116">
-        <v>-30</v>
-      </c>
-      <c r="C27" s="125">
-        <v>60</v>
-      </c>
-      <c r="D27" s="117">
-        <v>-90</v>
-      </c>
-      <c r="E27" s="128">
-        <v>59.5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="124">
-        <v>100</v>
-      </c>
-      <c r="B28" s="116">
-        <v>-30</v>
-      </c>
-      <c r="C28" s="125">
-        <v>-45</v>
-      </c>
-      <c r="D28" s="117">
-        <v>-48</v>
-      </c>
-      <c r="E28" s="128">
-        <v>-44.7</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="124">
-        <v>101</v>
-      </c>
-      <c r="B29" s="116">
-        <v>-30</v>
-      </c>
-      <c r="C29" s="125">
-        <v>-15</v>
-      </c>
-      <c r="D29" s="117">
-        <v>-33.5</v>
-      </c>
-      <c r="E29" s="128">
-        <v>-14.8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="124">
-        <v>102</v>
-      </c>
-      <c r="B30" s="116">
-        <v>-30</v>
-      </c>
-      <c r="C30" s="125">
-        <v>15</v>
-      </c>
-      <c r="D30" s="117">
-        <v>-34</v>
-      </c>
-      <c r="E30" s="128">
-        <v>16.7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="124">
-        <v>103</v>
-      </c>
-      <c r="B31" s="116">
-        <v>-30</v>
-      </c>
-      <c r="C31" s="125">
-        <v>45</v>
-      </c>
-      <c r="D31" s="117">
-        <v>-50</v>
-      </c>
-      <c r="E31" s="128">
-        <v>45.1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="124">
-        <v>85</v>
-      </c>
-      <c r="B32" s="116">
-        <v>-25</v>
-      </c>
-      <c r="C32" s="125">
-        <v>0</v>
-      </c>
-      <c r="D32" s="117">
-        <v>-25</v>
-      </c>
-      <c r="E32" s="128">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="B32" s="116"/>
+      <c r="C32" s="125"/>
+      <c r="D32" s="116"/>
+      <c r="E32" s="125"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="124">
-        <v>119</v>
-      </c>
-      <c r="B33" s="116">
-        <v>-20</v>
-      </c>
-      <c r="C33" s="125">
-        <v>0</v>
-      </c>
-      <c r="D33" s="117">
-        <v>-20</v>
-      </c>
-      <c r="E33" s="128">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="124">
-        <v>24</v>
-      </c>
-      <c r="B34" s="116">
-        <v>-15</v>
-      </c>
-      <c r="C34" s="125">
-        <v>75</v>
-      </c>
-      <c r="D34" s="117">
-        <v>-91</v>
-      </c>
-      <c r="E34" s="128">
-        <v>73.8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="124">
-        <v>37</v>
-      </c>
-      <c r="B35" s="116">
-        <v>-15</v>
-      </c>
-      <c r="C35" s="125">
-        <v>-30</v>
-      </c>
-      <c r="D35" s="117">
-        <v>-20</v>
-      </c>
-      <c r="E35" s="128">
-        <v>-27.8</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="124">
-        <v>38</v>
-      </c>
-      <c r="B36" s="116">
-        <v>-15</v>
-      </c>
-      <c r="C36" s="125">
-        <v>0</v>
-      </c>
-      <c r="D36" s="117">
-        <v>-15</v>
-      </c>
-      <c r="E36" s="128">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="124">
-        <v>39</v>
-      </c>
-      <c r="B37" s="116">
-        <v>-15</v>
-      </c>
-      <c r="C37" s="125">
-        <v>30</v>
-      </c>
-      <c r="D37" s="117">
-        <v>-19.5</v>
-      </c>
-      <c r="E37" s="128">
-        <v>31.7</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="124">
-        <v>40</v>
-      </c>
-      <c r="B38" s="116">
-        <v>-15</v>
-      </c>
-      <c r="C38" s="125">
-        <v>60</v>
-      </c>
-      <c r="D38" s="117">
-        <v>-34.5</v>
-      </c>
-      <c r="E38" s="128">
-        <v>60.4</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="A39" s="124">
-        <v>41</v>
-      </c>
-      <c r="B39" s="116">
-        <v>-15</v>
-      </c>
-      <c r="C39" s="125">
-        <v>120</v>
-      </c>
-      <c r="D39" s="117">
-        <v>-157</v>
-      </c>
-      <c r="E39" s="128">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="A40" s="124">
-        <v>70</v>
-      </c>
-      <c r="B40" s="116">
-        <v>-15</v>
-      </c>
-      <c r="C40" s="125">
-        <v>-45</v>
-      </c>
-      <c r="D40" s="117">
-        <v>-23</v>
-      </c>
-      <c r="E40" s="128">
-        <v>-43.4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="A41" s="124">
-        <v>71</v>
-      </c>
-      <c r="B41" s="116">
-        <v>-15</v>
-      </c>
-      <c r="C41" s="125">
-        <v>-15</v>
-      </c>
-      <c r="D41" s="117">
-        <v>-17</v>
-      </c>
-      <c r="E41" s="128">
-        <v>-14.7</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="A42" s="124">
-        <v>72</v>
-      </c>
-      <c r="B42" s="116">
-        <v>-15</v>
-      </c>
-      <c r="C42" s="125">
-        <v>15</v>
-      </c>
-      <c r="D42" s="117">
-        <v>-17</v>
-      </c>
-      <c r="E42" s="128">
-        <v>15.9</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="A43" s="124">
-        <v>73</v>
-      </c>
-      <c r="B43" s="116">
-        <v>-15</v>
-      </c>
-      <c r="C43" s="125">
-        <v>45</v>
-      </c>
-      <c r="D43" s="117">
-        <v>-25.5</v>
-      </c>
-      <c r="E43" s="128">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
-      <c r="A44" s="124">
-        <v>86</v>
-      </c>
-      <c r="B44" s="116">
-        <v>-10</v>
-      </c>
-      <c r="C44" s="125">
-        <v>0</v>
-      </c>
-      <c r="D44" s="117">
-        <v>-10</v>
-      </c>
-      <c r="E44" s="128">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
-      <c r="A45" s="124">
-        <v>120</v>
-      </c>
-      <c r="B45" s="116">
-        <v>-5</v>
-      </c>
-      <c r="C45" s="125">
-        <v>0</v>
-      </c>
-      <c r="D45" s="117">
-        <v>-5</v>
-      </c>
-      <c r="E45" s="128">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
-      <c r="A46" s="124">
-        <v>9</v>
-      </c>
-      <c r="B46" s="116">
-        <v>0</v>
-      </c>
-      <c r="C46" s="125">
-        <v>-30</v>
-      </c>
-      <c r="D46" s="117">
-        <v>0</v>
-      </c>
-      <c r="E46" s="128">
-        <v>-30.3</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
-      <c r="A47" s="124">
-        <v>10</v>
-      </c>
-      <c r="B47" s="116">
-        <v>0</v>
-      </c>
-      <c r="C47" s="125">
-        <v>0</v>
-      </c>
-      <c r="D47" s="117">
-        <v>0</v>
-      </c>
-      <c r="E47" s="128">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="A48" s="124">
-        <v>11</v>
-      </c>
-      <c r="B48" s="116">
-        <v>0</v>
-      </c>
-      <c r="C48" s="125">
-        <v>30</v>
-      </c>
-      <c r="D48" s="117">
-        <v>0</v>
-      </c>
-      <c r="E48" s="128">
-        <v>30.4</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
-      <c r="A49" s="124">
-        <v>12</v>
-      </c>
-      <c r="B49" s="116">
-        <v>0</v>
-      </c>
-      <c r="C49" s="125">
-        <v>60</v>
-      </c>
-      <c r="D49" s="117">
-        <v>0</v>
-      </c>
-      <c r="E49" s="128">
-        <v>60.3</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
-      <c r="A50" s="124">
-        <v>13</v>
-      </c>
-      <c r="B50" s="116">
-        <v>0</v>
-      </c>
-      <c r="C50" s="125">
-        <v>90</v>
-      </c>
-      <c r="D50" s="117">
-        <v>0</v>
-      </c>
-      <c r="E50" s="128">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
-      <c r="A51" s="124">
-        <v>14</v>
-      </c>
-      <c r="B51" s="116">
-        <v>0</v>
-      </c>
-      <c r="C51" s="125">
-        <v>120</v>
-      </c>
-      <c r="D51" s="117">
-        <v>0</v>
-      </c>
-      <c r="E51" s="128">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
-      <c r="A52" s="124">
-        <v>52</v>
-      </c>
-      <c r="B52" s="116">
-        <v>0</v>
-      </c>
-      <c r="C52" s="125">
-        <v>-40</v>
-      </c>
-      <c r="D52" s="117">
-        <v>0</v>
-      </c>
-      <c r="E52" s="128">
-        <v>-40.200000000000003</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5">
-      <c r="A53" s="124">
-        <v>53</v>
-      </c>
-      <c r="B53" s="116">
-        <v>0</v>
-      </c>
-      <c r="C53" s="125">
-        <v>-25</v>
-      </c>
-      <c r="D53" s="117">
-        <v>0</v>
-      </c>
-      <c r="E53" s="128">
-        <v>-24.8</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5">
-      <c r="A54" s="124">
-        <v>54</v>
-      </c>
-      <c r="B54" s="116">
-        <v>0</v>
-      </c>
-      <c r="C54" s="125">
-        <v>-10</v>
-      </c>
-      <c r="D54" s="117">
-        <v>0</v>
-      </c>
-      <c r="E54" s="128">
-        <v>-9.9</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5">
-      <c r="A55" s="124">
-        <v>55</v>
-      </c>
-      <c r="B55" s="116">
-        <v>0</v>
-      </c>
-      <c r="C55" s="125">
-        <v>5</v>
-      </c>
-      <c r="D55" s="117">
-        <v>0</v>
-      </c>
-      <c r="E55" s="128">
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5">
-      <c r="A56" s="124">
-        <v>56</v>
-      </c>
-      <c r="B56" s="116">
-        <v>0</v>
-      </c>
-      <c r="C56" s="125">
-        <v>20</v>
-      </c>
-      <c r="D56" s="117">
-        <v>0</v>
-      </c>
-      <c r="E56" s="128">
-        <v>20.3</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5">
-      <c r="A57" s="124">
-        <v>57</v>
-      </c>
-      <c r="B57" s="116">
-        <v>0</v>
-      </c>
-      <c r="C57" s="125">
-        <v>35</v>
-      </c>
-      <c r="D57" s="117">
-        <v>0</v>
-      </c>
-      <c r="E57" s="128">
-        <v>36.5</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5">
-      <c r="A58" s="124">
-        <v>90</v>
-      </c>
-      <c r="B58" s="116">
-        <v>0</v>
-      </c>
-      <c r="C58" s="125">
-        <v>-35</v>
-      </c>
-      <c r="D58" s="117">
-        <v>0</v>
-      </c>
-      <c r="E58" s="128">
-        <v>-34.9</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5">
-      <c r="A59" s="124">
-        <v>91</v>
-      </c>
-      <c r="B59" s="116">
-        <v>0</v>
-      </c>
-      <c r="C59" s="125">
-        <v>-20</v>
-      </c>
-      <c r="D59" s="117">
-        <v>0</v>
-      </c>
-      <c r="E59" s="128">
-        <v>-19.600000000000001</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5">
-      <c r="A60" s="124">
-        <v>92</v>
-      </c>
-      <c r="B60" s="116">
-        <v>0</v>
-      </c>
-      <c r="C60" s="125">
-        <v>-5</v>
-      </c>
-      <c r="D60" s="117">
-        <v>0</v>
-      </c>
-      <c r="E60" s="128">
-        <v>-5.8</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5">
-      <c r="A61" s="124">
-        <v>93</v>
-      </c>
-      <c r="B61" s="116">
-        <v>0</v>
-      </c>
-      <c r="C61" s="125">
-        <v>10</v>
-      </c>
-      <c r="D61" s="117">
-        <v>0</v>
-      </c>
-      <c r="E61" s="128">
-        <v>10.3</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5">
-      <c r="A62" s="124">
-        <v>94</v>
-      </c>
-      <c r="B62" s="116">
-        <v>0</v>
-      </c>
-      <c r="C62" s="125">
-        <v>25</v>
-      </c>
-      <c r="D62" s="117">
-        <v>0</v>
-      </c>
-      <c r="E62" s="128">
-        <v>25.3</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5">
-      <c r="A63" s="124">
-        <v>95</v>
-      </c>
-      <c r="B63" s="116">
-        <v>0</v>
-      </c>
-      <c r="C63" s="125">
-        <v>40</v>
-      </c>
-      <c r="D63" s="117">
-        <v>0</v>
-      </c>
-      <c r="E63" s="128">
-        <v>40.700000000000003</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5">
-      <c r="A64" s="124">
-        <v>104</v>
-      </c>
-      <c r="B64" s="116">
-        <v>0</v>
-      </c>
-      <c r="C64" s="125">
-        <v>-45</v>
-      </c>
-      <c r="D64" s="117">
-        <v>0</v>
-      </c>
-      <c r="E64" s="128">
-        <v>-45.3</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5">
-      <c r="A65" s="124">
-        <v>105</v>
-      </c>
-      <c r="B65" s="116">
-        <v>0</v>
-      </c>
-      <c r="C65" s="125">
-        <v>-15</v>
-      </c>
-      <c r="D65" s="117">
-        <v>0</v>
-      </c>
-      <c r="E65" s="128">
-        <v>-14.8</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5">
-      <c r="A66" s="124">
-        <v>106</v>
-      </c>
-      <c r="B66" s="116">
-        <v>0</v>
-      </c>
-      <c r="C66" s="125">
-        <v>15</v>
-      </c>
-      <c r="D66" s="117">
-        <v>0</v>
-      </c>
-      <c r="E66" s="128">
-        <v>15.3</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5">
-      <c r="A67" s="124">
-        <v>107</v>
-      </c>
-      <c r="B67" s="116">
-        <v>0</v>
-      </c>
-      <c r="C67" s="125">
-        <v>45</v>
-      </c>
-      <c r="D67" s="117">
-        <v>0</v>
-      </c>
-      <c r="E67" s="128">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5">
-      <c r="A68" s="124">
-        <v>108</v>
-      </c>
-      <c r="B68" s="116">
-        <v>0</v>
-      </c>
-      <c r="C68" s="125">
-        <v>75</v>
-      </c>
-      <c r="D68" s="117">
-        <v>0</v>
-      </c>
-      <c r="E68" s="128">
-        <v>74.5</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5">
-      <c r="A69" s="124">
-        <v>109</v>
-      </c>
-      <c r="B69" s="116">
-        <v>0</v>
-      </c>
-      <c r="C69" s="125">
-        <v>105</v>
-      </c>
-      <c r="D69" s="117">
-        <v>0</v>
-      </c>
-      <c r="E69" s="128">
-        <v>105.4</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5">
-      <c r="A70" s="124">
-        <v>87</v>
-      </c>
-      <c r="B70" s="116">
-        <v>5</v>
-      </c>
-      <c r="C70" s="125">
-        <v>0</v>
-      </c>
-      <c r="D70" s="117">
-        <v>5</v>
-      </c>
-      <c r="E70" s="128">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5">
-      <c r="A71" s="124">
-        <v>121</v>
-      </c>
-      <c r="B71" s="116">
-        <v>10</v>
-      </c>
-      <c r="C71" s="125">
-        <v>0</v>
-      </c>
-      <c r="D71" s="117">
-        <v>10</v>
-      </c>
-      <c r="E71" s="128">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5">
-      <c r="A72" s="124">
-        <v>25</v>
-      </c>
-      <c r="B72" s="116">
-        <v>15</v>
-      </c>
-      <c r="C72" s="125">
-        <v>75</v>
-      </c>
-      <c r="D72" s="117">
-        <v>90</v>
-      </c>
-      <c r="E72" s="128">
-        <v>74.400000000000006</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5">
-      <c r="A73" s="124">
-        <v>42</v>
-      </c>
-      <c r="B73" s="116">
-        <v>15</v>
-      </c>
-      <c r="C73" s="125">
-        <v>-30</v>
-      </c>
-      <c r="D73" s="117">
-        <v>17</v>
-      </c>
-      <c r="E73" s="128">
-        <v>-27.3</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5">
-      <c r="A74" s="124">
-        <v>43</v>
-      </c>
-      <c r="B74" s="116">
-        <v>15</v>
-      </c>
-      <c r="C74" s="125">
-        <v>0</v>
-      </c>
-      <c r="D74" s="117">
-        <v>15</v>
-      </c>
-      <c r="E74" s="128">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5">
-      <c r="A75" s="124">
-        <v>44</v>
-      </c>
-      <c r="B75" s="116">
-        <v>15</v>
-      </c>
-      <c r="C75" s="125">
-        <v>30</v>
-      </c>
-      <c r="D75" s="117">
-        <v>19.5</v>
-      </c>
-      <c r="E75" s="128">
-        <v>32.1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5">
-      <c r="A76" s="124">
-        <v>45</v>
-      </c>
-      <c r="B76" s="116">
-        <v>15</v>
-      </c>
-      <c r="C76" s="125">
-        <v>60</v>
-      </c>
-      <c r="D76" s="117">
-        <v>150</v>
-      </c>
-      <c r="E76" s="128">
-        <v>56.5</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5">
-      <c r="A77" s="124">
-        <v>46</v>
-      </c>
-      <c r="B77" s="116">
-        <v>15</v>
-      </c>
-      <c r="C77" s="125">
-        <v>120</v>
-      </c>
-      <c r="D77" s="117">
-        <v>157</v>
-      </c>
-      <c r="E77" s="128">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5">
-      <c r="A78" s="124">
-        <v>74</v>
-      </c>
-      <c r="B78" s="116">
-        <v>15</v>
-      </c>
-      <c r="C78" s="125">
-        <v>-45</v>
-      </c>
-      <c r="D78" s="117">
-        <v>21</v>
-      </c>
-      <c r="E78" s="128">
-        <v>-43.4</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5">
-      <c r="A79" s="124">
-        <v>75</v>
-      </c>
-      <c r="B79" s="116">
-        <v>15</v>
-      </c>
-      <c r="C79" s="125">
-        <v>-15</v>
-      </c>
-      <c r="D79" s="117">
-        <v>16</v>
-      </c>
-      <c r="E79" s="128">
-        <v>-14.5</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5">
-      <c r="A80" s="124">
-        <v>76</v>
-      </c>
-      <c r="B80" s="116">
-        <v>15</v>
-      </c>
-      <c r="C80" s="125">
-        <v>15</v>
-      </c>
-      <c r="D80" s="117">
-        <v>15</v>
-      </c>
-      <c r="E80" s="128">
-        <v>16.2</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5">
-      <c r="A81" s="124">
-        <v>77</v>
-      </c>
-      <c r="B81" s="116">
-        <v>15</v>
-      </c>
-      <c r="C81" s="125">
-        <v>45</v>
-      </c>
-      <c r="D81" s="117">
-        <v>24.5</v>
-      </c>
-      <c r="E81" s="128">
-        <v>47.6</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5">
-      <c r="A82" s="124">
-        <v>88</v>
-      </c>
-      <c r="B82" s="116">
-        <v>20</v>
-      </c>
-      <c r="C82" s="125">
-        <v>0</v>
-      </c>
-      <c r="D82" s="117">
-        <v>20</v>
-      </c>
-      <c r="E82" s="128">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5">
-      <c r="A83" s="124">
-        <v>122</v>
-      </c>
-      <c r="B83" s="116">
-        <v>25</v>
-      </c>
-      <c r="C83" s="125">
-        <v>0</v>
-      </c>
-      <c r="D83" s="117">
-        <v>25</v>
-      </c>
-      <c r="E83" s="128">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5">
-      <c r="A84" s="124">
-        <v>15</v>
-      </c>
-      <c r="B84" s="116">
-        <v>30</v>
-      </c>
-      <c r="C84" s="125">
-        <v>-30</v>
-      </c>
-      <c r="D84" s="117">
-        <v>34</v>
-      </c>
-      <c r="E84" s="128">
-        <v>-27.5</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5">
-      <c r="A85" s="124">
-        <v>16</v>
-      </c>
-      <c r="B85" s="116">
-        <v>30</v>
-      </c>
-      <c r="C85" s="125">
-        <v>0</v>
-      </c>
-      <c r="D85" s="117">
-        <v>30</v>
-      </c>
-      <c r="E85" s="128">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5">
-      <c r="A86" s="124">
-        <v>17</v>
-      </c>
-      <c r="B86" s="116">
-        <v>30</v>
-      </c>
-      <c r="C86" s="125">
-        <v>30</v>
-      </c>
-      <c r="D86" s="117">
-        <v>38</v>
-      </c>
-      <c r="E86" s="128">
-        <v>30.4</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5">
-      <c r="A87" s="124">
-        <v>18</v>
-      </c>
-      <c r="B87" s="116">
-        <v>30</v>
-      </c>
-      <c r="C87" s="125">
-        <v>60</v>
-      </c>
-      <c r="D87" s="117">
-        <v>88</v>
-      </c>
-      <c r="E87" s="128">
-        <v>59.2</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5">
-      <c r="A88" s="124">
-        <v>110</v>
-      </c>
-      <c r="B88" s="116">
-        <v>30</v>
-      </c>
-      <c r="C88" s="125">
-        <v>-45</v>
-      </c>
-      <c r="D88" s="117">
-        <v>45</v>
-      </c>
-      <c r="E88" s="128">
-        <v>-45.2</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5">
-      <c r="A89" s="124">
-        <v>111</v>
-      </c>
-      <c r="B89" s="116">
-        <v>30</v>
-      </c>
-      <c r="C89" s="125">
-        <v>-15</v>
-      </c>
-      <c r="D89" s="117">
         <v>31</v>
       </c>
-      <c r="E89" s="128">
-        <v>-14.9</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5">
-      <c r="A90" s="124">
-        <v>112</v>
-      </c>
-      <c r="B90" s="116">
-        <v>30</v>
-      </c>
-      <c r="C90" s="125">
-        <v>15</v>
-      </c>
-      <c r="D90" s="117">
-        <v>33</v>
-      </c>
-      <c r="E90" s="128">
-        <v>15.8</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5">
-      <c r="A91" s="124">
-        <v>113</v>
-      </c>
-      <c r="B91" s="116">
-        <v>30</v>
-      </c>
-      <c r="C91" s="125">
-        <v>45</v>
-      </c>
-      <c r="D91" s="117">
-        <v>47</v>
-      </c>
-      <c r="E91" s="128">
-        <v>43.7</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5">
-      <c r="A92" s="124">
-        <v>89</v>
-      </c>
-      <c r="B92" s="116">
-        <v>35</v>
-      </c>
-      <c r="C92" s="125">
-        <v>0</v>
-      </c>
-      <c r="D92" s="117">
-        <v>35</v>
-      </c>
-      <c r="E92" s="128">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5">
-      <c r="A93" s="124">
-        <v>123</v>
-      </c>
-      <c r="B93" s="116">
-        <v>40</v>
-      </c>
-      <c r="C93" s="125">
-        <v>0</v>
-      </c>
-      <c r="D93" s="117">
-        <v>40</v>
-      </c>
-      <c r="E93" s="128">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5">
-      <c r="A94" s="124">
-        <v>47</v>
-      </c>
-      <c r="B94" s="116">
-        <v>45</v>
-      </c>
-      <c r="C94" s="125">
-        <v>-30</v>
-      </c>
-      <c r="D94" s="117">
-        <v>56</v>
-      </c>
-      <c r="E94" s="128">
-        <v>-30.3</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5">
-      <c r="A95" s="124">
-        <v>48</v>
-      </c>
-      <c r="B95" s="116">
-        <v>45</v>
-      </c>
-      <c r="C95" s="125">
-        <v>0</v>
-      </c>
-      <c r="D95" s="117">
-        <v>45</v>
-      </c>
-      <c r="E95" s="128">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5">
-      <c r="A96" s="124">
-        <v>49</v>
-      </c>
-      <c r="B96" s="116">
-        <v>45</v>
-      </c>
-      <c r="C96" s="125">
-        <v>30</v>
-      </c>
-      <c r="D96" s="117">
-        <v>55</v>
-      </c>
-      <c r="E96" s="128">
-        <v>30.6</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5">
-      <c r="A97" s="124">
-        <v>78</v>
-      </c>
-      <c r="B97" s="116">
-        <v>45</v>
-      </c>
-      <c r="C97" s="125">
-        <v>-45</v>
-      </c>
-      <c r="D97" s="117">
-        <v>72</v>
-      </c>
-      <c r="E97" s="128">
-        <v>-41.8</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5">
-      <c r="A98" s="124">
-        <v>79</v>
-      </c>
-      <c r="B98" s="116">
-        <v>45</v>
-      </c>
-      <c r="C98" s="125">
-        <v>-15</v>
-      </c>
-      <c r="D98" s="117">
-        <v>48</v>
-      </c>
-      <c r="E98" s="128">
-        <v>-15.5</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5">
-      <c r="A99" s="124">
-        <v>80</v>
-      </c>
-      <c r="B99" s="116">
-        <v>45</v>
-      </c>
-      <c r="C99" s="125">
-        <v>15</v>
-      </c>
-      <c r="D99" s="117">
-        <v>49.5</v>
-      </c>
-      <c r="E99" s="128">
-        <v>15.2</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5">
-      <c r="A100" s="124">
-        <v>81</v>
-      </c>
-      <c r="B100" s="116">
-        <v>45</v>
-      </c>
-      <c r="C100" s="125">
-        <v>45</v>
-      </c>
-      <c r="D100" s="117">
-        <v>65.5</v>
-      </c>
-      <c r="E100" s="128">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5">
-      <c r="A101" s="124">
-        <v>19</v>
-      </c>
-      <c r="B101" s="116">
-        <v>60</v>
-      </c>
-      <c r="C101" s="125">
-        <v>-30</v>
-      </c>
-      <c r="D101" s="117">
-        <v>92.5</v>
-      </c>
-      <c r="E101" s="128">
-        <v>-29.3</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5">
-      <c r="A102" s="124">
-        <v>20</v>
-      </c>
-      <c r="B102" s="116">
-        <v>60</v>
-      </c>
-      <c r="C102" s="125">
-        <v>0</v>
-      </c>
-      <c r="D102" s="117">
-        <v>62</v>
-      </c>
-      <c r="E102" s="128">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5">
-      <c r="A103" s="124">
-        <v>21</v>
-      </c>
-      <c r="B103" s="116">
-        <v>60</v>
-      </c>
-      <c r="C103" s="125">
-        <v>30</v>
-      </c>
-      <c r="D103" s="117">
-        <v>90</v>
-      </c>
-      <c r="E103" s="128">
-        <v>31.1</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5">
-      <c r="A104" s="124">
-        <v>114</v>
-      </c>
-      <c r="B104" s="116">
-        <v>60</v>
-      </c>
-      <c r="C104" s="125">
-        <v>-15</v>
-      </c>
-      <c r="D104" s="117">
-        <v>64</v>
-      </c>
-      <c r="E104" s="128">
-        <v>-14.1</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5">
-      <c r="A105" s="124">
-        <v>115</v>
-      </c>
-      <c r="B105" s="116">
-        <v>60</v>
-      </c>
-      <c r="C105" s="125">
-        <v>15</v>
-      </c>
-      <c r="D105" s="117">
-        <v>65</v>
-      </c>
-      <c r="E105" s="128">
-        <v>16.8</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5">
-      <c r="A106" s="124">
-        <v>50</v>
-      </c>
-      <c r="B106" s="116">
-        <v>75</v>
-      </c>
-      <c r="C106" s="125">
-        <v>0</v>
-      </c>
-      <c r="D106" s="117">
-        <v>72</v>
-      </c>
-      <c r="E106" s="128">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5">
-      <c r="A107" s="124">
-        <v>82</v>
-      </c>
-      <c r="B107" s="116">
-        <v>75</v>
-      </c>
-      <c r="C107" s="125">
-        <v>-15</v>
-      </c>
-      <c r="D107" s="117">
-        <v>91.5</v>
-      </c>
-      <c r="E107" s="128">
-        <v>-13.9</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5">
-      <c r="A108" s="124">
-        <v>83</v>
-      </c>
-      <c r="B108" s="116">
-        <v>75</v>
-      </c>
-      <c r="C108" s="125">
-        <v>15</v>
-      </c>
-      <c r="D108" s="117">
-        <v>91</v>
-      </c>
-      <c r="E108" s="128">
-        <v>15.7</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5">
-      <c r="A109" s="124">
-        <v>22</v>
-      </c>
-      <c r="B109" s="116">
-        <v>90</v>
-      </c>
-      <c r="C109" s="125">
-        <v>0</v>
-      </c>
-      <c r="D109" s="117">
-        <v>91.5</v>
-      </c>
-      <c r="E109" s="128">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5">
-      <c r="A110" s="124">
-        <v>51</v>
-      </c>
-      <c r="B110" s="116">
-        <v>105</v>
-      </c>
-      <c r="C110" s="125">
-        <v>0</v>
-      </c>
-      <c r="D110" s="117">
-        <v>105.5</v>
-      </c>
-      <c r="E110" s="128">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5">
-      <c r="A111" s="124">
-        <v>23</v>
-      </c>
-      <c r="B111" s="116">
-        <v>120</v>
-      </c>
-      <c r="C111" s="125">
-        <v>0</v>
-      </c>
-      <c r="D111" s="117">
-        <v>120</v>
-      </c>
-      <c r="E111" s="128">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5">
-      <c r="A112" s="124">
-        <v>116</v>
-      </c>
-      <c r="B112" s="116">
-        <v>120</v>
-      </c>
-      <c r="C112" s="125">
-        <v>-15</v>
-      </c>
-      <c r="D112" s="117">
-        <v>115.5</v>
-      </c>
-      <c r="E112" s="128">
-        <v>-13.7</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" ht="16" thickBot="1">
-      <c r="A113" s="129">
-        <v>117</v>
-      </c>
-      <c r="B113" s="130">
-        <v>120</v>
-      </c>
-      <c r="C113" s="131">
-        <v>15</v>
-      </c>
-      <c r="D113" s="132">
-        <v>115.5</v>
-      </c>
-      <c r="E113" s="133">
-        <v>15.9</v>
-      </c>
+      <c r="B33" s="116"/>
+      <c r="C33" s="125"/>
+      <c r="D33" s="116"/>
+      <c r="E33" s="125"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="124"/>
+      <c r="B34" s="116"/>
+      <c r="C34" s="125"/>
+      <c r="D34" s="116"/>
+      <c r="E34" s="125"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="124"/>
+      <c r="B35" s="116"/>
+      <c r="C35" s="125"/>
+      <c r="D35" s="117"/>
+      <c r="E35" s="126"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="124"/>
+      <c r="B36" s="116"/>
+      <c r="C36" s="125"/>
+      <c r="D36" s="117"/>
+      <c r="E36" s="126"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="124"/>
+      <c r="B37" s="116"/>
+      <c r="C37" s="125"/>
+      <c r="D37" s="117"/>
+      <c r="E37" s="126"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="124"/>
+      <c r="B38" s="116"/>
+      <c r="C38" s="125"/>
+      <c r="D38" s="117"/>
+      <c r="E38" s="126"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="124"/>
+      <c r="B39" s="116"/>
+      <c r="C39" s="125"/>
+      <c r="D39" s="117"/>
+      <c r="E39" s="126"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="124"/>
+      <c r="B40" s="116"/>
+      <c r="C40" s="125"/>
+      <c r="D40" s="117"/>
+      <c r="E40" s="126"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="124"/>
+      <c r="B41" s="116"/>
+      <c r="C41" s="125"/>
+      <c r="D41" s="117"/>
+      <c r="E41" s="126"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="124"/>
+      <c r="B42" s="116"/>
+      <c r="C42" s="125"/>
+      <c r="D42" s="117"/>
+      <c r="E42" s="126"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="124"/>
+      <c r="B43" s="116"/>
+      <c r="C43" s="125"/>
+      <c r="D43" s="117"/>
+      <c r="E43" s="126"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="124"/>
+      <c r="B44" s="116"/>
+      <c r="C44" s="125"/>
+      <c r="D44" s="117"/>
+      <c r="E44" s="126"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="124"/>
+      <c r="B45" s="116"/>
+      <c r="C45" s="125"/>
+      <c r="D45" s="117"/>
+      <c r="E45" s="126"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="124"/>
+      <c r="B46" s="116"/>
+      <c r="C46" s="125"/>
+      <c r="D46" s="117"/>
+      <c r="E46" s="126"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="124"/>
+      <c r="B47" s="116"/>
+      <c r="C47" s="125"/>
+      <c r="D47" s="117"/>
+      <c r="E47" s="126"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="124"/>
+      <c r="B48" s="116"/>
+      <c r="C48" s="125"/>
+      <c r="D48" s="117"/>
+      <c r="E48" s="126"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="124"/>
+      <c r="B49" s="116"/>
+      <c r="C49" s="125"/>
+      <c r="D49" s="117"/>
+      <c r="E49" s="126"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="124"/>
+      <c r="B50" s="116"/>
+      <c r="C50" s="125"/>
+      <c r="D50" s="117"/>
+      <c r="E50" s="126"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="124"/>
+      <c r="B51" s="116"/>
+      <c r="C51" s="125"/>
+      <c r="D51" s="117"/>
+      <c r="E51" s="126"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="124"/>
+      <c r="B52" s="116"/>
+      <c r="C52" s="125"/>
+      <c r="D52" s="117"/>
+      <c r="E52" s="126"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="124"/>
+      <c r="B53" s="116"/>
+      <c r="C53" s="125"/>
+      <c r="D53" s="117"/>
+      <c r="E53" s="126"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="124"/>
+      <c r="B54" s="116"/>
+      <c r="C54" s="125"/>
+      <c r="D54" s="117"/>
+      <c r="E54" s="126"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="124"/>
+      <c r="B55" s="116"/>
+      <c r="C55" s="125"/>
+      <c r="D55" s="117"/>
+      <c r="E55" s="126"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="124"/>
+      <c r="B56" s="116"/>
+      <c r="C56" s="125"/>
+      <c r="D56" s="117"/>
+      <c r="E56" s="126"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="124"/>
+      <c r="B57" s="116"/>
+      <c r="C57" s="125"/>
+      <c r="D57" s="117"/>
+      <c r="E57" s="126"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="124"/>
+      <c r="B58" s="116"/>
+      <c r="C58" s="125"/>
+      <c r="D58" s="117"/>
+      <c r="E58" s="126"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="124"/>
+      <c r="B59" s="116"/>
+      <c r="C59" s="125"/>
+      <c r="D59" s="117"/>
+      <c r="E59" s="126"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="124"/>
+      <c r="B60" s="116"/>
+      <c r="C60" s="125"/>
+      <c r="D60" s="117"/>
+      <c r="E60" s="126"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="124"/>
+      <c r="B61" s="116"/>
+      <c r="C61" s="125"/>
+      <c r="D61" s="117"/>
+      <c r="E61" s="126"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="124"/>
+      <c r="B62" s="116"/>
+      <c r="C62" s="125"/>
+      <c r="D62" s="117"/>
+      <c r="E62" s="126"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="124"/>
+      <c r="B63" s="116"/>
+      <c r="C63" s="125"/>
+      <c r="D63" s="117"/>
+      <c r="E63" s="126"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="124"/>
+      <c r="B64" s="116"/>
+      <c r="C64" s="125"/>
+      <c r="D64" s="117"/>
+      <c r="E64" s="126"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="124"/>
+      <c r="B65" s="116"/>
+      <c r="C65" s="125"/>
+      <c r="D65" s="117"/>
+      <c r="E65" s="126"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="124"/>
+      <c r="B66" s="116"/>
+      <c r="C66" s="125"/>
+      <c r="D66" s="117"/>
+      <c r="E66" s="126"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="124"/>
+      <c r="B67" s="116"/>
+      <c r="C67" s="125"/>
+      <c r="D67" s="117"/>
+      <c r="E67" s="126"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="124"/>
+      <c r="B68" s="116"/>
+      <c r="C68" s="125"/>
+      <c r="D68" s="117"/>
+      <c r="E68" s="126"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="124"/>
+      <c r="B69" s="116"/>
+      <c r="C69" s="125"/>
+      <c r="D69" s="117"/>
+      <c r="E69" s="126"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="124"/>
+      <c r="B70" s="116"/>
+      <c r="C70" s="125"/>
+      <c r="D70" s="117"/>
+      <c r="E70" s="126"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="124"/>
+      <c r="B71" s="116"/>
+      <c r="C71" s="125"/>
+      <c r="D71" s="117"/>
+      <c r="E71" s="126"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="124"/>
+      <c r="B72" s="116"/>
+      <c r="C72" s="125"/>
+      <c r="D72" s="117"/>
+      <c r="E72" s="126"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="124"/>
+      <c r="B73" s="116"/>
+      <c r="C73" s="125"/>
+      <c r="D73" s="117"/>
+      <c r="E73" s="126"/>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="124"/>
+      <c r="B74" s="116"/>
+      <c r="C74" s="125"/>
+      <c r="D74" s="117"/>
+      <c r="E74" s="126"/>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="124"/>
+      <c r="B75" s="116"/>
+      <c r="C75" s="125"/>
+      <c r="D75" s="117"/>
+      <c r="E75" s="126"/>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="124"/>
+      <c r="B76" s="116"/>
+      <c r="C76" s="125"/>
+      <c r="D76" s="117"/>
+      <c r="E76" s="126"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="124"/>
+      <c r="B77" s="116"/>
+      <c r="C77" s="125"/>
+      <c r="D77" s="117"/>
+      <c r="E77" s="126"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="124"/>
+      <c r="B78" s="116"/>
+      <c r="C78" s="125"/>
+      <c r="D78" s="117"/>
+      <c r="E78" s="126"/>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="124"/>
+      <c r="B79" s="116"/>
+      <c r="C79" s="125"/>
+      <c r="D79" s="117"/>
+      <c r="E79" s="126"/>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="124"/>
+      <c r="B80" s="116"/>
+      <c r="C80" s="125"/>
+      <c r="D80" s="117"/>
+      <c r="E80" s="126"/>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="124"/>
+      <c r="B81" s="116"/>
+      <c r="C81" s="125"/>
+      <c r="D81" s="117"/>
+      <c r="E81" s="126"/>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="124"/>
+      <c r="B82" s="116"/>
+      <c r="C82" s="125"/>
+      <c r="D82" s="117"/>
+      <c r="E82" s="126"/>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="124"/>
+      <c r="B83" s="116"/>
+      <c r="C83" s="125"/>
+      <c r="D83" s="117"/>
+      <c r="E83" s="126"/>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="124"/>
+      <c r="B84" s="116"/>
+      <c r="C84" s="125"/>
+      <c r="D84" s="117"/>
+      <c r="E84" s="126"/>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="124"/>
+      <c r="B85" s="116"/>
+      <c r="C85" s="125"/>
+      <c r="D85" s="117"/>
+      <c r="E85" s="126"/>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="124"/>
+      <c r="B86" s="116"/>
+      <c r="C86" s="125"/>
+      <c r="D86" s="117"/>
+      <c r="E86" s="126"/>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="124"/>
+      <c r="B87" s="116"/>
+      <c r="C87" s="125"/>
+      <c r="D87" s="117"/>
+      <c r="E87" s="126"/>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="124"/>
+      <c r="B88" s="116"/>
+      <c r="C88" s="125"/>
+      <c r="D88" s="117"/>
+      <c r="E88" s="126"/>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="124"/>
+      <c r="B89" s="116"/>
+      <c r="C89" s="125"/>
+      <c r="D89" s="117"/>
+      <c r="E89" s="126"/>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="124"/>
+      <c r="B90" s="116"/>
+      <c r="C90" s="125"/>
+      <c r="D90" s="117"/>
+      <c r="E90" s="126"/>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="124"/>
+      <c r="B91" s="116"/>
+      <c r="C91" s="125"/>
+      <c r="D91" s="117"/>
+      <c r="E91" s="126"/>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="124"/>
+      <c r="B92" s="116"/>
+      <c r="C92" s="125"/>
+      <c r="D92" s="117"/>
+      <c r="E92" s="126"/>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="124"/>
+      <c r="B93" s="116"/>
+      <c r="C93" s="125"/>
+      <c r="D93" s="117"/>
+      <c r="E93" s="126"/>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" s="124"/>
+      <c r="B94" s="116"/>
+      <c r="C94" s="125"/>
+      <c r="D94" s="117"/>
+      <c r="E94" s="126"/>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" s="124"/>
+      <c r="B95" s="116"/>
+      <c r="C95" s="125"/>
+      <c r="D95" s="117"/>
+      <c r="E95" s="126"/>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" s="124"/>
+      <c r="B96" s="116"/>
+      <c r="C96" s="125"/>
+      <c r="D96" s="117"/>
+      <c r="E96" s="126"/>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" s="124"/>
+      <c r="B97" s="116"/>
+      <c r="C97" s="125"/>
+      <c r="D97" s="117"/>
+      <c r="E97" s="126"/>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" s="124"/>
+      <c r="B98" s="116"/>
+      <c r="C98" s="125"/>
+      <c r="D98" s="117"/>
+      <c r="E98" s="126"/>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" s="124"/>
+      <c r="B99" s="116"/>
+      <c r="C99" s="125"/>
+      <c r="D99" s="117"/>
+      <c r="E99" s="126"/>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" s="124"/>
+      <c r="B100" s="116"/>
+      <c r="C100" s="125"/>
+      <c r="D100" s="117"/>
+      <c r="E100" s="126"/>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" s="124"/>
+      <c r="B101" s="116"/>
+      <c r="C101" s="125"/>
+      <c r="D101" s="117"/>
+      <c r="E101" s="126"/>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" s="124"/>
+      <c r="B102" s="116"/>
+      <c r="C102" s="125"/>
+      <c r="D102" s="117"/>
+      <c r="E102" s="126"/>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" s="124"/>
+      <c r="B103" s="116"/>
+      <c r="C103" s="125"/>
+      <c r="D103" s="117"/>
+      <c r="E103" s="126"/>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" s="124"/>
+      <c r="B104" s="116"/>
+      <c r="C104" s="125"/>
+      <c r="D104" s="117"/>
+      <c r="E104" s="126"/>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" s="124"/>
+      <c r="B105" s="116"/>
+      <c r="C105" s="125"/>
+      <c r="D105" s="117"/>
+      <c r="E105" s="126"/>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" s="124"/>
+      <c r="B106" s="116"/>
+      <c r="C106" s="125"/>
+      <c r="D106" s="117"/>
+      <c r="E106" s="126"/>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" s="124"/>
+      <c r="B107" s="116"/>
+      <c r="C107" s="125"/>
+      <c r="D107" s="117"/>
+      <c r="E107" s="126"/>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" s="124"/>
+      <c r="B108" s="116"/>
+      <c r="C108" s="125"/>
+      <c r="D108" s="117"/>
+      <c r="E108" s="126"/>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" s="124"/>
+      <c r="B109" s="116"/>
+      <c r="C109" s="125"/>
+      <c r="D109" s="117"/>
+      <c r="E109" s="126"/>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" s="124"/>
+      <c r="B110" s="116"/>
+      <c r="C110" s="125"/>
+      <c r="D110" s="117"/>
+      <c r="E110" s="126"/>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" s="124"/>
+      <c r="B111" s="116"/>
+      <c r="C111" s="125"/>
+      <c r="D111" s="117"/>
+      <c r="E111" s="126"/>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" s="124"/>
+      <c r="B112" s="116"/>
+      <c r="C112" s="125"/>
+      <c r="D112" s="117"/>
+      <c r="E112" s="126"/>
+    </row>
+    <row r="113" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A113" s="127"/>
+      <c r="B113" s="128"/>
+      <c r="C113" s="129"/>
+      <c r="D113" s="130"/>
+      <c r="E113" s="131"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>

</xml_diff>